<commit_message>
Add infile and inside parameters to festivals-up;oad.
</commit_message>
<xml_diff>
--- a/festivals-upload/demo.xlsx
+++ b/festivals-upload/demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Festival" sheetId="1" state="visible" r:id="rId2"/>
@@ -3216,7 +3216,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
@@ -3347,8 +3347,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3413,7 +3413,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="B2:B3 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3567,8 +3567,8 @@
   </sheetPr>
   <dimension ref="A1:F149"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A55" activeCellId="1" sqref="B2:B3 A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6261,8 +6261,8 @@
   </sheetPr>
   <dimension ref="A1:S437"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M147" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O153" activeCellId="1" sqref="B2:B3 O153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24102,7 +24102,7 @@
   <dimension ref="A3:A17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B2:B3 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24166,7 +24166,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="289" zoomScaleNormal="289" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="B2:B3 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>